<commit_message>
verdicts added; code rearrangement
</commit_message>
<xml_diff>
--- a/public/scripts/users.xlsx
+++ b/public/scripts/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\TestSystemPack\TestSystem\public\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37C780B-92EA-413F-9527-B803448F63ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C3DCE-E07E-4CF8-BA8D-BA9C9D127A94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="612" windowWidth="23304" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>Login</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>u10001</t>
-  </si>
-  <si>
-    <t>u10002</t>
   </si>
   <si>
     <t>Бабушкин Андрей Иванович</t>
@@ -613,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,349 +635,349 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>